<commit_message>
Paypal brain tree and attributes in box type
</commit_message>
<xml_diff>
--- a/proVidioETG/testDate/GiftCertificateCodes.xlsx
+++ b/proVidioETG/testDate/GiftCertificateCodes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t xml:space="preserve">Codes</t>
   </si>
@@ -110,31 +110,22 @@
     <t xml:space="preserve">codes</t>
   </si>
   <si>
-    <t xml:space="preserve">OSZITLVRRPIITTAA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZLGHSJJQFDMQGWYQ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JMTMKLKFVLZKJMSJ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FYKWSLFHLCAOHADY </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIWTWDQGMGCPYLKQ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JMMWDZMZJWHMLCJT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CWFSORQWDTWFKDYY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GKDFRMMLTSOPZSQP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LPACKMITQCGHPFVJ </t>
+    <t xml:space="preserve">LZOKCKSKITLTMZPH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAHZTYLVDRPJLSRR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLSJSZWQDIYJRCTH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WOODRMOLGSQHYYGF </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZYAJYSVDTCRCTWYD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">YOJOKYYVHQLMIJFW </t>
   </si>
 </sst>
 </file>
@@ -433,10 +424,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -479,24 +470,6 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0"/>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
commit on aug 22
</commit_message>
<xml_diff>
--- a/proVidioETG/testDate/GiftCertificateCodes.xlsx
+++ b/proVidioETG/testDate/GiftCertificateCodes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t xml:space="preserve">Codes</t>
   </si>
@@ -113,28 +113,55 @@
     <t xml:space="preserve">LZOKCKSKITLTMZPH </t>
   </si>
   <si>
-    <t xml:space="preserve">LAHZTYLVDRPJLSRR</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> OMVVTHALOOQOSFSC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TVQLWACCZLARHCKO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HTCTWPLVZHPPWAFP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TZLAJCTOKSPOYYDF </t>
+    <t xml:space="preserve">KOSGYMSSFYPCYWOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LQOCOOOFTAIDSHKI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZZZGODTJQZYMOJSC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFKGVCSMTIGAJPVD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KVJOKCKHKAPFPYWP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRIFAQDZCGSIDFMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YOJOKYYVHQLMIJFW </t>
   </si>
   <si>
     <t xml:space="preserve">FSZYIHDVIMJMHYLD </t>
   </si>
   <si>
-    <t xml:space="preserve">ZYAJYSVDTCRCTWYD </t>
-  </si>
-  <si>
-    <t xml:space="preserve">YOJOKYYVHQLMIJFW </t>
+    <t xml:space="preserve">LQHZDFQRHAKAMGHC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SJGYSIVIODHSPDOJ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LQKDYKARZKYTKSZY </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DQLCKSFTYIYQVOLP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VYCSTQKCMWTWMPQR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IHZQRCKDZPKIWMMJ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIDHDYRQMVIMCQIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTPFHAWJWPHPJTZL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KTCAKAPJKZDLOARK </t>
   </si>
 </sst>
 </file>
@@ -144,7 +171,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -180,12 +207,6 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -246,7 +267,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -439,10 +460,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -466,43 +487,98 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>36</v>
+      <c r="A9" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
salesforce and brain tree paypal
</commit_message>
<xml_diff>
--- a/proVidioETG/testDate/GiftCertificateCodes.xlsx
+++ b/proVidioETG/testDate/GiftCertificateCodes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t xml:space="preserve">Codes</t>
   </si>
@@ -113,15 +113,6 @@
     <t xml:space="preserve">LZOKCKSKITLTMZPH </t>
   </si>
   <si>
-    <t xml:space="preserve">KOSGYMSSFYPCYWOS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LQOCOOOFTAIDSHKI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZZZGODTJQZYMOJSC </t>
-  </si>
-  <si>
     <t xml:space="preserve">MFKGVCSMTIGAJPVD </t>
   </si>
   <si>
@@ -129,12 +120,6 @@
   </si>
   <si>
     <t xml:space="preserve">IRIFAQDZCGSIDFMP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YOJOKYYVHQLMIJFW </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FSZYIHDVIMJMHYLD </t>
   </si>
   <si>
     <t xml:space="preserve">LQHZDFQRHAKAMGHC </t>
@@ -250,7 +235,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -265,10 +250,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -460,10 +441,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -481,104 +462,79 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>